<commit_message>
correccion de equipos en red
</commit_message>
<xml_diff>
--- a/reporte mensual programador.xlsx
+++ b/reporte mensual programador.xlsx
@@ -31401,8 +31401,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15:T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31898,7 +31898,7 @@
       <c r="P15" s="106"/>
       <c r="Q15" s="108"/>
       <c r="R15" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="S15" s="106"/>
       <c r="T15" s="108"/>

</xml_diff>